<commit_message>
HW4: Q3 times added.
</commit_message>
<xml_diff>
--- a/HW4/times.xlsx
+++ b/HW4/times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Radin\Documents\MCP\HW4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA053A4-8A36-4563-A797-BD722102EFAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E8B656-79B2-4971-86F5-5CEA3D072C9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>serial</t>
   </si>
@@ -357,9 +357,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -504,9 +506,156 @@
         <v>2.3078166297362888</v>
       </c>
     </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>1024</v>
+      </c>
+      <c r="C11">
+        <v>4096</v>
+      </c>
+      <c r="E11">
+        <v>1024</v>
+      </c>
+      <c r="F11">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0.33892099999999997</v>
+      </c>
+      <c r="C12">
+        <v>23.258996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>0.16855100000000001</v>
+      </c>
+      <c r="C13">
+        <v>12.561260000000001</v>
+      </c>
+      <c r="E13">
+        <f>B12/B13</f>
+        <v>2.0107919858084493</v>
+      </c>
+      <c r="F13">
+        <f>C12/C13</f>
+        <v>1.8516451375100904</v>
+      </c>
+      <c r="H13">
+        <f>AVERAGE(E13:F13)</f>
+        <v>1.9312185616592699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>8.2139000000000004E-2</v>
+      </c>
+      <c r="C14">
+        <v>5.782565</v>
+      </c>
+      <c r="E14">
+        <f>B12/B14</f>
+        <v>4.1261885340702946</v>
+      </c>
+      <c r="F14">
+        <f>C12/C14</f>
+        <v>4.0222627847676593</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14:H17" si="2">AVERAGE(E14:F14)</f>
+        <v>4.0742256594189765</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>6.5322000000000005E-2</v>
+      </c>
+      <c r="C15">
+        <v>4.4164570000000003</v>
+      </c>
+      <c r="E15">
+        <f>B12/B15</f>
+        <v>5.188466366614616</v>
+      </c>
+      <c r="F15">
+        <f>C12/C15</f>
+        <v>5.266437780329345</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>5.22745207347198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>6.9593000000000002E-2</v>
+      </c>
+      <c r="C16">
+        <v>4.2484320000000002</v>
+      </c>
+      <c r="E16">
+        <f>B12/B16</f>
+        <v>4.8700444010173429</v>
+      </c>
+      <c r="F16">
+        <f>C12/C16</f>
+        <v>5.4747247925822986</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>5.1723845967998212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>6.8673999999999999E-2</v>
+      </c>
+      <c r="C17">
+        <v>4.2780319999999996</v>
+      </c>
+      <c r="E17">
+        <f>B12/B17</f>
+        <v>4.9352156565803647</v>
+      </c>
+      <c r="F17">
+        <f>C12/C17</f>
+        <v>5.436844792184818</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>5.1860302243825913</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="H1:L1"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>